<commit_message>
Add spec parts 8 and 9 in Spanish
</commit_message>
<xml_diff>
--- a/Specification/Spanish/Editable source images/Imágenes Spec Parte 9 - Formatos de archivo.xlsx
+++ b/Specification/Spanish/Editable source images/Imágenes Spec Parte 9 - Formatos de archivo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="7980" windowHeight="9855" activeTab="8"/>
+    <workbookView xWindow="600" yWindow="60" windowWidth="7980" windowHeight="9855"/>
   </bookViews>
   <sheets>
     <sheet name="Signatures" sheetId="9" r:id="rId1"/>
@@ -677,7 +677,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="53">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1348,6 +1348,19 @@
       <top/>
       <bottom style="thick">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1550,10 +1563,19 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1595,6 +1617,15 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1607,25 +1638,7 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1930,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:R12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2073,10 +2086,10 @@
       <c r="O10" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="P10" s="76" t="s">
+      <c r="P10" s="101" t="s">
         <v>72</v>
       </c>
-      <c r="Q10" s="77" t="s">
+      <c r="Q10" s="76" t="s">
         <v>73</v>
       </c>
       <c r="R10" s="18"/>
@@ -2146,25 +2159,25 @@
     </row>
     <row r="3" spans="2:22" s="9" customFormat="1" ht="30" customHeight="1">
       <c r="B3" s="17"/>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="84" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="81"/>
-      <c r="S3" s="81"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="R3" s="84"/>
+      <c r="S3" s="84"/>
       <c r="T3" s="18"/>
     </row>
     <row r="4" spans="2:22" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -2273,18 +2286,18 @@
       <c r="K6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="82" t="s">
+      <c r="L6" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="82" t="s">
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="Q6" s="83"/>
-      <c r="R6" s="83"/>
-      <c r="S6" s="84"/>
+      <c r="Q6" s="86"/>
+      <c r="R6" s="86"/>
+      <c r="S6" s="87"/>
       <c r="T6" s="18"/>
       <c r="V6" s="9" t="s">
         <v>45</v>
@@ -2525,30 +2538,30 @@
       <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="82" t="s">
+      <c r="D11" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="83"/>
-      <c r="F11" s="83"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="82" t="s">
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="83"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="91" t="s">
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="M11" s="92"/>
-      <c r="N11" s="92"/>
-      <c r="O11" s="93"/>
-      <c r="P11" s="91" t="s">
+      <c r="M11" s="98"/>
+      <c r="N11" s="98"/>
+      <c r="O11" s="99"/>
+      <c r="P11" s="97" t="s">
         <v>86</v>
       </c>
-      <c r="Q11" s="92"/>
-      <c r="R11" s="92"/>
-      <c r="S11" s="93"/>
+      <c r="Q11" s="98"/>
+      <c r="R11" s="98"/>
+      <c r="S11" s="99"/>
       <c r="T11" s="18"/>
     </row>
     <row r="12" spans="2:22" ht="30" customHeight="1" thickBot="1">
@@ -2556,30 +2569,30 @@
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="85" t="s">
+      <c r="D12" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="88" t="s">
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="85" t="s">
+      <c r="I12" s="92"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="93"/>
+      <c r="L12" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="M12" s="86"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="85" t="s">
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="90"/>
+      <c r="P12" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="Q12" s="86"/>
-      <c r="R12" s="86"/>
-      <c r="S12" s="87"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="90"/>
       <c r="T12" s="18"/>
     </row>
     <row r="13" spans="2:22" ht="30" customHeight="1" thickBot="1">
@@ -2587,28 +2600,28 @@
       <c r="C13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="85" t="s">
+      <c r="D13" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="85" t="s">
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="87"/>
-      <c r="L13" s="99" t="s">
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="94" t="s">
         <v>137</v>
       </c>
-      <c r="M13" s="100"/>
-      <c r="N13" s="100"/>
-      <c r="O13" s="100"/>
-      <c r="P13" s="100"/>
-      <c r="Q13" s="100"/>
-      <c r="R13" s="100"/>
-      <c r="S13" s="101"/>
+      <c r="M13" s="95"/>
+      <c r="N13" s="95"/>
+      <c r="O13" s="95"/>
+      <c r="P13" s="95"/>
+      <c r="Q13" s="95"/>
+      <c r="R13" s="95"/>
+      <c r="S13" s="96"/>
       <c r="T13" s="18"/>
     </row>
     <row r="14" spans="2:22" ht="30" customHeight="1" thickBot="1">
@@ -2640,19 +2653,19 @@
         <v>22</v>
       </c>
       <c r="F15" s="19"/>
-      <c r="G15" s="78" t="s">
+      <c r="G15" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="79"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="80"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="82"/>
+      <c r="Q15" s="83"/>
       <c r="R15" s="19"/>
       <c r="S15" s="19"/>
       <c r="T15" s="18"/>
@@ -2686,19 +2699,19 @@
         <v>22</v>
       </c>
       <c r="F17" s="19"/>
-      <c r="G17" s="78" t="s">
+      <c r="G17" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="79"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="79"/>
-      <c r="P17" s="79"/>
-      <c r="Q17" s="80"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="82"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="83"/>
       <c r="R17" s="19"/>
       <c r="S17" s="19"/>
       <c r="T17" s="18"/>
@@ -2756,7 +2769,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2913,7 +2926,7 @@
   <dimension ref="B3:J20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3237,12 +3250,12 @@
       <c r="J5" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="82" t="s">
+      <c r="K5" s="85" t="s">
         <v>121</v>
       </c>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="84"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="87"/>
       <c r="O5" s="13"/>
       <c r="P5" s="25"/>
       <c r="Q5" s="25"/>
@@ -3375,18 +3388,18 @@
       <c r="J9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="82" t="s">
+      <c r="K9" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="84"/>
-      <c r="O9" s="82" t="s">
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="85" t="s">
         <v>116</v>
       </c>
-      <c r="P9" s="83"/>
-      <c r="Q9" s="83"/>
-      <c r="R9" s="84"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="86"/>
+      <c r="R9" s="87"/>
       <c r="S9" s="18"/>
       <c r="U9" s="9" t="s">
         <v>39</v>
@@ -3507,12 +3520,12 @@
       <c r="J13" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="82" t="s">
+      <c r="K13" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="L13" s="83"/>
-      <c r="M13" s="83"/>
-      <c r="N13" s="84"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="87"/>
       <c r="O13" s="13"/>
       <c r="P13" s="25"/>
       <c r="Q13" s="25"/>
@@ -3561,7 +3574,7 @@
   <dimension ref="B1:AH12"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3764,12 +3777,12 @@
       <c r="J5" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="82" t="s">
+      <c r="K5" s="85" t="s">
         <v>121</v>
       </c>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="84"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="87"/>
       <c r="O5" s="18"/>
       <c r="Q5" s="17"/>
       <c r="R5" s="26" t="s">
@@ -3796,18 +3809,18 @@
       <c r="Y5" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="Z5" s="82" t="s">
+      <c r="Z5" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="AA5" s="83"/>
-      <c r="AB5" s="83"/>
-      <c r="AC5" s="84"/>
-      <c r="AD5" s="82" t="s">
+      <c r="AA5" s="86"/>
+      <c r="AB5" s="86"/>
+      <c r="AC5" s="87"/>
+      <c r="AD5" s="85" t="s">
         <v>116</v>
       </c>
-      <c r="AE5" s="83"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="84"/>
+      <c r="AE5" s="86"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="87"/>
       <c r="AH5" s="18"/>
     </row>
     <row r="6" spans="2:34" ht="22.5" customHeight="1">
@@ -3945,12 +3958,12 @@
       <c r="J11" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="82" t="s">
+      <c r="K11" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
-      <c r="N11" s="84"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="87"/>
       <c r="O11" s="18"/>
     </row>
     <row r="12" spans="2:34" ht="22.5" customHeight="1">
@@ -3988,7 +4001,7 @@
   <dimension ref="B3:J20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4138,7 +4151,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:P12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -4168,7 +4183,7 @@
     </row>
     <row r="3" spans="2:16" ht="30" customHeight="1" thickBot="1">
       <c r="B3" s="44"/>
-      <c r="C3" s="95" t="s">
+      <c r="C3" s="77" t="s">
         <v>123</v>
       </c>
       <c r="D3" s="45"/>
@@ -4256,7 +4271,7 @@
     </row>
     <row r="9" spans="2:16" ht="30" customHeight="1" thickBot="1">
       <c r="M9" s="17"/>
-      <c r="N9" s="96" t="s">
+      <c r="N9" s="78" t="s">
         <v>124</v>
       </c>
       <c r="O9" s="19"/>
@@ -4264,10 +4279,10 @@
     </row>
     <row r="10" spans="2:16" ht="30" customHeight="1" thickBot="1">
       <c r="M10" s="17"/>
-      <c r="N10" s="97" t="s">
+      <c r="N10" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="O10" s="98" t="s">
+      <c r="O10" s="80" t="s">
         <v>125</v>
       </c>
       <c r="P10" s="18"/>
@@ -4301,7 +4316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -4420,77 +4435,77 @@
     <row r="7" spans="2:14" ht="11.25" customHeight="1">
       <c r="B7" s="17"/>
       <c r="C7" s="51"/>
-      <c r="D7" s="94" t="s">
+      <c r="D7" s="100" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
       <c r="M7" s="68"/>
       <c r="N7" s="18"/>
     </row>
     <row r="8" spans="2:14" ht="11.25" customHeight="1">
       <c r="B8" s="17"/>
       <c r="C8" s="70"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+      <c r="K8" s="100"/>
+      <c r="L8" s="100"/>
       <c r="M8" s="68"/>
       <c r="N8" s="18"/>
     </row>
     <row r="9" spans="2:14" ht="11.25" customHeight="1">
       <c r="B9" s="17"/>
       <c r="C9" s="51"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="100"/>
+      <c r="J9" s="100"/>
+      <c r="K9" s="100"/>
+      <c r="L9" s="100"/>
       <c r="M9" s="68"/>
       <c r="N9" s="18"/>
     </row>
     <row r="10" spans="2:14" ht="11.25" customHeight="1">
       <c r="B10" s="17"/>
       <c r="C10" s="70"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="94"/>
-      <c r="L10" s="94"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="100"/>
+      <c r="H10" s="100"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="100"/>
+      <c r="K10" s="100"/>
+      <c r="L10" s="100"/>
       <c r="M10" s="68"/>
       <c r="N10" s="18"/>
     </row>
     <row r="11" spans="2:14" ht="11.25" customHeight="1">
       <c r="B11" s="17"/>
       <c r="C11" s="51"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="94"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="100"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="100"/>
+      <c r="I11" s="100"/>
+      <c r="J11" s="100"/>
+      <c r="K11" s="100"/>
+      <c r="L11" s="100"/>
       <c r="M11" s="68"/>
       <c r="N11" s="18"/>
     </row>

</xml_diff>